<commit_message>
Got Meta-Data working fully
Good news: This is now working fully. I even updated the excel sheet so it prevents you from entering duplicate data under title and ID. Now, the code will automatically update the created json file so it is just an array. Then I iterate over the entire array, creating a file for each scenario. The file name is based off of the ID (which is why I forced it to be unique). So Event 5 will have a file name "Scenario5.json". I left the old version in though, so if we wanted to use the array notation and just have one large file, we can.
</commit_message>
<xml_diff>
--- a/Bystander Intervention/MetaData/Book3.xlsx
+++ b/Bystander Intervention/MetaData/Book3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Documents\Games\SeniorDesign480\Bystander Intervention\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{844B8FB0-804F-439F-B4B7-4046A1A5EC61}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D523DBEF-4AE7-40E0-BDEE-82BA67DC8D66}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12810" xr2:uid="{6CCB2488-0D6D-4EC9-A2A8-43151E4FAC94}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +461,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -477,6 +477,15 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Duplicate Scene ID" error="This scene ID already exists. You are either using the wrong ID, or you need to update an existing entry." sqref="A2:A564" xr:uid="{B34EEDD6-D531-4CA9-8623-416BEE6A7F5F}">
+      <formula1>COUNTIF($A:$A,A2)=1</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Duplicate Title" error="You have entered a duplicate Title. This scene either already exists, and you need to find it, or you need to create a more meaningful (and unique) title." sqref="B1:B1048576" xr:uid="{953A7014-D9FA-41DA-B1BF-3E2CB17FD53F}">
+      <formula1>COUNTIF($B:$B,B1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>